<commit_message>
Distinguished between 'events' and 'questions'; added a deck of generic questions to pick from; added the option to include custom questions with each event.
</commit_message>
<xml_diff>
--- a/data/firstHistoricClimateEvents.xlsx
+++ b/data/firstHistoricClimateEvents.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachel/Documents/Projects/Climate-Conversations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/projects/climate_conversations/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24660" windowHeight="13600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
   <si>
     <t>start year</t>
   </si>
@@ -297,6 +297,12 @@
   </si>
   <si>
     <t>The world's first mass-produced hybrid electric vehicle, the Prius, was released in Japan.</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>Has your region considered implementing a carbon tax?</t>
   </si>
 </sst>
 </file>
@@ -657,11 +663,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB999"/>
+  <dimension ref="A1:AC999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -672,11 +678,11 @@
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" customWidth="1"/>
     <col min="7" max="7" width="85.83203125" customWidth="1"/>
-    <col min="8" max="8" width="43.5" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="8" max="9" width="43.5" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -701,10 +707,12 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -723,8 +731,9 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
-    </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="AC1" s="2"/>
+    </row>
+    <row r="2" spans="1:29" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1930</v>
       </c>
@@ -740,8 +749,9 @@
       <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>1930</v>
       </c>
@@ -751,8 +761,9 @@
       <c r="H3" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" ht="26" x14ac:dyDescent="0.15">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>1952</v>
       </c>
@@ -765,8 +776,9 @@
       <c r="H4" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>1957</v>
       </c>
@@ -791,8 +803,9 @@
       <c r="H5" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" ht="26" x14ac:dyDescent="0.15">
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>1958</v>
       </c>
@@ -802,8 +815,9 @@
       <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" ht="26" x14ac:dyDescent="0.15">
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>1962</v>
       </c>
@@ -825,8 +839,9 @@
       <c r="H7" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>1963</v>
       </c>
@@ -851,8 +866,9 @@
       <c r="H8" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>1970</v>
       </c>
@@ -877,8 +893,9 @@
       <c r="H9" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>1970</v>
       </c>
@@ -897,8 +914,9 @@
       <c r="H10" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" ht="26" x14ac:dyDescent="0.15">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:29" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>1970</v>
       </c>
@@ -914,8 +932,9 @@
       <c r="H11" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" ht="26" x14ac:dyDescent="0.15">
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:29" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>1970</v>
       </c>
@@ -928,8 +947,9 @@
       <c r="H12" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:29" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>1974</v>
       </c>
@@ -939,8 +959,9 @@
       <c r="H13" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:29" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>1980</v>
       </c>
@@ -954,7 +975,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:29" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>1982</v>
       </c>
@@ -970,8 +991,9 @@
       <c r="H15" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:29" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>1982</v>
       </c>
@@ -984,8 +1006,9 @@
       <c r="H16" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>1985</v>
       </c>
@@ -1010,8 +1033,9 @@
       <c r="H17" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>1987</v>
       </c>
@@ -1021,8 +1045,9 @@
       <c r="H18" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>1988</v>
       </c>
@@ -1032,8 +1057,9 @@
       <c r="H19" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>1989</v>
       </c>
@@ -1046,8 +1072,9 @@
       <c r="H20" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>1990</v>
       </c>
@@ -1060,8 +1087,9 @@
       <c r="H21" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>1991</v>
       </c>
@@ -1083,8 +1111,9 @@
       <c r="H22" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>1992</v>
       </c>
@@ -1097,8 +1126,9 @@
       <c r="H23" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>1993</v>
       </c>
@@ -1117,8 +1147,9 @@
       <c r="H24" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>1995</v>
       </c>
@@ -1131,8 +1162,9 @@
       <c r="H25" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>1997</v>
       </c>
@@ -1145,8 +1177,9 @@
       <c r="H26" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>1999</v>
       </c>
@@ -1156,8 +1189,9 @@
       <c r="H27" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>2001</v>
       </c>
@@ -1167,8 +1201,9 @@
       <c r="H28" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>2001</v>
       </c>
@@ -1178,8 +1213,9 @@
       <c r="H29" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>2003</v>
       </c>
@@ -1189,8 +1225,9 @@
       <c r="H30" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>2005</v>
       </c>
@@ -1206,8 +1243,9 @@
       <c r="H31" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>2007</v>
       </c>
@@ -1232,8 +1270,9 @@
       <c r="H32" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <v>2007</v>
       </c>
@@ -1243,8 +1282,9 @@
       <c r="H33" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <v>2007</v>
       </c>
@@ -1257,8 +1297,9 @@
       <c r="H34" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <v>2013</v>
       </c>
@@ -1268,8 +1309,9 @@
       <c r="H35" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>2008</v>
       </c>
@@ -1279,8 +1321,9 @@
       <c r="H36" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <v>1954</v>
       </c>
@@ -1290,8 +1333,9 @@
       <c r="H37" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <v>2010</v>
       </c>
@@ -1301,8 +1345,9 @@
       <c r="H38" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>2014</v>
       </c>
@@ -1312,8 +1357,9 @@
       <c r="H39" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="26" x14ac:dyDescent="0.15">
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>1991</v>
       </c>
@@ -1323,8 +1369,9 @@
       <c r="H40" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>1990</v>
       </c>
@@ -1334,8 +1381,9 @@
       <c r="H41" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="3">
         <v>2008</v>
       </c>
@@ -1345,8 +1393,11 @@
       <c r="H42" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I42" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="3">
         <v>2013</v>
       </c>
@@ -1356,8 +1407,9 @@
       <c r="H43" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="3">
         <v>1976</v>
       </c>
@@ -1367,8 +1419,9 @@
       <c r="H44" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="3">
         <v>1997</v>
       </c>
@@ -1378,14 +1431,15 @@
       <c r="H45" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="7:7" ht="13" x14ac:dyDescent="0.15">

</xml_diff>